<commit_message>
Changing to coord args
</commit_message>
<xml_diff>
--- a/xl/tests/test1.xlsx
+++ b/xl/tests/test1.xlsx
@@ -4,20 +4,20 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="0" firstSheet="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="990" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
+    <workbookView activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
-  <calcPr calcId="124519" fullCalcOnLoad="1" iterate="0" iterateCount="100" iterateDelta="0.0001" refMode="A1"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="7">
-  <si>
-    <t>Hello World</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="13">
+  <si>
+    <t>Testing</t>
   </si>
   <si>
     <t>A</t>
@@ -32,10 +32,28 @@
     <t>X</t>
   </si>
   <si>
+    <t>CHI</t>
+  </si>
+  <si>
     <t>Y</t>
   </si>
   <si>
+    <t>ALPHA</t>
+  </si>
+  <si>
+    <t>BETA</t>
+  </si>
+  <si>
+    <t>GAMMA</t>
+  </si>
+  <si>
+    <t>PSI</t>
+  </si>
+  <si>
     <t>Z</t>
+  </si>
+  <si>
+    <t>OMEGA</t>
   </si>
 </sst>
 </file>
@@ -43,52 +61,24 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="6">
+  <fonts count="2">
     <font>
       <name val="Calibri"/>
-      <charset val="1"/>
       <family val="2"/>
-      <color rgb="FF000000"/>
+      <color theme="1"/>
       <sz val="11"/>
-    </font>
-    <font>
-      <name val="Arial"/>
-      <family val="0"/>
-      <sz val="10"/>
-    </font>
-    <font>
-      <name val="Arial"/>
-      <family val="0"/>
-      <sz val="10"/>
-    </font>
-    <font>
-      <name val="Arial"/>
-      <family val="0"/>
-      <sz val="10"/>
-    </font>
-    <font>
-      <name val="Cambria"/>
-      <charset val="1"/>
-      <family val="1"/>
-      <b val="1"/>
-      <sz val="11"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <b val="1"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill>
-        <fgColor rgb="80808080"/>
-        <bgColor rgb="80808080"/>
-      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -105,40 +95,19 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="6">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
+  <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="general" vertical="bottom"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="4" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="general" vertical="bottom"/>
-    </xf>
+  <cellXfs count="2">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="0" fillId="2" fontId="5" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="3" fontId="5" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf applyAlignment="1" borderId="0" fillId="2" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="6">
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
-    <cellStyle builtinId="3" name="Comma" xfId="1"/>
-    <cellStyle builtinId="6" name="Comma [0]" xfId="2"/>
-    <cellStyle builtinId="4" name="Currency" xfId="3"/>
-    <cellStyle builtinId="7" name="Currency [0]" xfId="4"/>
-    <cellStyle builtinId="5" name="Percent" xfId="5"/>
+  <cellStyles count="1">
+    <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
   </cellStyles>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
 </styleSheet>
 </file>
 
@@ -427,27 +396,53 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr filterMode="0">
+  <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr fitToPage="0"/>
+    <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="1" rightToLeft="0" showFormulas="0" showGridLines="1" showOutlineSymbols="1" showRowColHeaders="1" showZeros="1" tabSelected="1" topLeftCell="A1" view="normal" windowProtection="0" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="C15" activeCellId="0" pane="topLeft" sqref="C15"/>
+    <sheetView workbookViewId="0">
+      <pane activePane="bottomRight" state="frozen" topLeftCell="B2" xSplit="1" ySplit="1"/>
+      <selection pane="topRight"/>
+      <selection pane="bottomLeft"/>
+      <selection activeCell="A1" pane="bottomRight" sqref="A1"/>
+      <selection activeCell="A1" pane="bottomLeft" sqref="A1"/>
+      <selection activeCell="A1" pane="bottomRight" sqref="A1"/>
+      <selection activeCell="A1" pane="bottomLeft" sqref="A1"/>
+      <selection activeCell="A1" pane="bottomRight" sqref="A1"/>
+      <selection activeCell="A1" pane="bottomLeft" sqref="A1"/>
+      <selection activeCell="A1" pane="bottomRight" sqref="A1"/>
+      <selection activeCell="A1" pane="bottomLeft" sqref="A1"/>
+      <selection activeCell="A1" pane="bottomRight" sqref="A1"/>
+      <selection activeCell="A1" pane="bottomLeft" sqref="A1"/>
+      <selection activeCell="A1" pane="bottomRight" sqref="A1"/>
+      <selection activeCell="A1" pane="bottomLeft" sqref="A1"/>
+      <selection activeCell="A1" pane="bottomRight" sqref="A1"/>
+      <selection activeCell="A1" pane="bottomLeft" sqref="A1"/>
+      <selection activeCell="A1" pane="bottomRight" sqref="A1"/>
+      <selection activeCell="A1" pane="bottomLeft" sqref="A1"/>
+      <selection activeCell="A1" pane="bottomRight" sqref="A1"/>
+      <selection activeCell="A1" pane="bottomLeft" sqref="A1"/>
+      <selection activeCell="A1" pane="bottomRight" sqref="A1"/>
+      <selection activeCell="A1" pane="bottomLeft" sqref="A1"/>
+      <selection activeCell="A1" pane="bottomRight" sqref="A1"/>
+      <selection activeCell="A1" pane="bottomLeft" sqref="A1"/>
+      <selection activeCell="A1" pane="bottomRight" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
   <cols>
-    <col customWidth="1" max="1025" min="1" style="2" width="8.570850202429151"/>
+    <col customWidth="1" max="1" min="1" width="9.9"/>
+    <col customWidth="1" max="2" min="2" width="25"/>
   </cols>
   <sheetData>
-    <row customHeight="1" ht="13.8" r="1" s="3" spans="1:3">
-      <c r="A1" s="5" t="s">
+    <row r="1" spans="1:7">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:7">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -458,24 +453,40 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:7">
       <c r="A3" t="s">
         <v>4</v>
       </c>
+      <c r="G3" s="1" t="s">
+        <v>5</v>
+      </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:7">
       <c r="A4" t="s">
-        <v>5</v>
+        <v>6</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:7">
       <c r="A5" t="s">
-        <v>6</v>
+        <v>11</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>
-  <printOptions gridLines="0" gridLinesSet="1" headings="0" horizontalCentered="0" verticalCentered="0"/>
-  <pageMargins bottom="1" footer="0.511805555555555" header="0.511805555555555" left="0.75" right="0.75" top="1"/>
-  <pageSetup blackAndWhite="0" copies="1" draft="0" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="1" scale="100" useFirstPageNumber="0" usePrinterDefaults="0" verticalDpi="300"/>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
More coordinate stuff, and block
</commit_message>
<xml_diff>
--- a/xl/tests/test1.xlsx
+++ b/xl/tests/test1.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="20">
   <si>
     <t>Testing</t>
   </si>
@@ -54,6 +54,27 @@
   </si>
   <si>
     <t>OMEGA</t>
+  </si>
+  <si>
+    <t>ACDC</t>
+  </si>
+  <si>
+    <t>BTO</t>
+  </si>
+  <si>
+    <t>Align Tech</t>
+  </si>
+  <si>
+    <t>Boeing</t>
+  </si>
+  <si>
+    <t>Citigroup</t>
+  </si>
+  <si>
+    <t>Audi</t>
+  </si>
+  <si>
+    <t>Buick</t>
   </si>
 </sst>
 </file>
@@ -400,14 +421,12 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane activePane="bottomRight" state="frozen" topLeftCell="B2" xSplit="1" ySplit="1"/>
+      <pane activePane="bottomRight" state="frozen" topLeftCell="b2" xSplit="1" ySplit="1"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection activeCell="A1" pane="bottomRight" sqref="A1"/>
-      <selection activeCell="A1" pane="bottomLeft" sqref="A1"/>
       <selection activeCell="A1" pane="bottomRight" sqref="A1"/>
       <selection activeCell="A1" pane="bottomLeft" sqref="A1"/>
       <selection activeCell="A1" pane="bottomRight" sqref="A1"/>
@@ -433,7 +452,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
   <cols>
-    <col customWidth="1" max="1" min="1" width="9.9"/>
+    <col customWidth="1" max="1" min="1" width="13.2"/>
     <col customWidth="1" max="2" min="2" width="25"/>
   </cols>
   <sheetData>
@@ -486,6 +505,37 @@
         <v>12</v>
       </c>
     </row>
+    <row r="6" spans="1:7"/>
+    <row r="7" spans="1:7"/>
+    <row r="8" spans="1:7"/>
+    <row r="9" spans="1:7"/>
+    <row r="10" spans="1:7">
+      <c r="A10" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="A11" t="s">
+        <v>15</v>
+      </c>
+      <c r="B11" t="s">
+        <v>16</v>
+      </c>
+      <c r="C11" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
+      <c r="A12" t="s">
+        <v>18</v>
+      </c>
+      <c r="B12" t="s">
+        <v>19</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>

</xml_diff>